<commit_message>
Updated on 6th June 2020
</commit_message>
<xml_diff>
--- a/SupportFiles/TestDaily_Test.xlsx
+++ b/SupportFiles/TestDaily_Test.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK53"/>
+  <dimension ref="A1:AK67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -860,7 +860,7 @@
         <v>0</v>
       </c>
       <c r="AB4">
-        <v>0</v>
+        <v>1434</v>
       </c>
       <c r="AC4">
         <v>0</v>
@@ -881,13 +881,13 @@
         <v>0</v>
       </c>
       <c r="AI4">
-        <v>0</v>
+        <v>678</v>
       </c>
       <c r="AJ4">
         <v>659</v>
       </c>
       <c r="AK4">
-        <v>27748</v>
+        <v>29860</v>
       </c>
     </row>
     <row r="5">
@@ -940,7 +940,7 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>4587</v>
       </c>
       <c r="R5">
         <v>9744</v>
@@ -973,7 +973,7 @@
         <v>0</v>
       </c>
       <c r="AB5">
-        <v>0</v>
+        <v>1434</v>
       </c>
       <c r="AC5">
         <v>0</v>
@@ -994,13 +994,13 @@
         <v>0</v>
       </c>
       <c r="AI5">
-        <v>0</v>
+        <v>678</v>
       </c>
       <c r="AJ5">
         <v>1042</v>
       </c>
       <c r="AK5">
-        <v>24149</v>
+        <v>30848</v>
       </c>
     </row>
     <row r="6">
@@ -1053,7 +1053,7 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>4587</v>
       </c>
       <c r="R6">
         <v>10221</v>
@@ -1086,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="AB6">
-        <v>0</v>
+        <v>1434</v>
       </c>
       <c r="AC6">
         <v>12279</v>
@@ -1107,13 +1107,13 @@
         <v>5255</v>
       </c>
       <c r="AI6">
-        <v>0</v>
+        <v>678</v>
       </c>
       <c r="AJ6">
         <v>1487</v>
       </c>
       <c r="AK6">
-        <v>66013</v>
+        <v>72712</v>
       </c>
     </row>
     <row r="7">
@@ -1166,7 +1166,7 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>4587</v>
       </c>
       <c r="R7">
         <v>10716</v>
@@ -1199,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="AB7">
-        <v>0</v>
+        <v>1434</v>
       </c>
       <c r="AC7">
         <v>12279</v>
@@ -1220,13 +1220,13 @@
         <v>5255</v>
       </c>
       <c r="AI7">
-        <v>0</v>
+        <v>678</v>
       </c>
       <c r="AJ7">
         <v>1301</v>
       </c>
       <c r="AK7">
-        <v>67995</v>
+        <v>74694</v>
       </c>
     </row>
     <row r="8">
@@ -1312,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="AB8">
-        <v>0</v>
+        <v>1434</v>
       </c>
       <c r="AC8">
         <v>17638</v>
@@ -1339,7 +1339,7 @@
         <v>1487</v>
       </c>
       <c r="AK8">
-        <v>94858</v>
+        <v>96292</v>
       </c>
     </row>
     <row r="9">
@@ -6425,6 +6425,1588 @@
       </c>
       <c r="AK53">
         <v>3046749</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2">
+        <v>43974</v>
+      </c>
+      <c r="B54">
+        <v>6677</v>
+      </c>
+      <c r="C54">
+        <v>292969</v>
+      </c>
+      <c r="D54">
+        <v>5206</v>
+      </c>
+      <c r="E54">
+        <v>60405</v>
+      </c>
+      <c r="F54">
+        <v>61220</v>
+      </c>
+      <c r="G54">
+        <v>3749</v>
+      </c>
+      <c r="H54">
+        <v>45522</v>
+      </c>
+      <c r="I54">
+        <v>382</v>
+      </c>
+      <c r="J54">
+        <v>165047</v>
+      </c>
+      <c r="K54">
+        <v>11945</v>
+      </c>
+      <c r="L54">
+        <v>178068</v>
+      </c>
+      <c r="M54">
+        <v>94035</v>
+      </c>
+      <c r="N54">
+        <v>25905</v>
+      </c>
+      <c r="O54">
+        <v>124074</v>
+      </c>
+      <c r="P54">
+        <v>45785</v>
+      </c>
+      <c r="Q54">
+        <v>196196</v>
+      </c>
+      <c r="R54">
+        <v>60443</v>
+      </c>
+      <c r="S54">
+        <v>5727</v>
+      </c>
+      <c r="T54">
+        <v>132769</v>
+      </c>
+      <c r="U54">
+        <v>348932</v>
+      </c>
+      <c r="V54">
+        <v>1706</v>
+      </c>
+      <c r="W54">
+        <v>3682</v>
+      </c>
+      <c r="X54">
+        <v>336</v>
+      </c>
+      <c r="Y54">
+        <v>1065</v>
+      </c>
+      <c r="Z54">
+        <v>118446</v>
+      </c>
+      <c r="AA54">
+        <v>6106</v>
+      </c>
+      <c r="AB54">
+        <v>63567</v>
+      </c>
+      <c r="AC54">
+        <v>303935</v>
+      </c>
+      <c r="AD54">
+        <v>1707</v>
+      </c>
+      <c r="AE54">
+        <v>397340</v>
+      </c>
+      <c r="AF54">
+        <v>23388</v>
+      </c>
+      <c r="AG54">
+        <v>18737</v>
+      </c>
+      <c r="AH54">
+        <v>217867</v>
+      </c>
+      <c r="AI54">
+        <v>19248</v>
+      </c>
+      <c r="AJ54">
+        <v>129608</v>
+      </c>
+      <c r="AK54">
+        <v>3171794</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2">
+        <v>43975</v>
+      </c>
+      <c r="B55">
+        <v>6677</v>
+      </c>
+      <c r="C55">
+        <v>304326</v>
+      </c>
+      <c r="D55">
+        <v>5206</v>
+      </c>
+      <c r="E55">
+        <v>60405</v>
+      </c>
+      <c r="F55">
+        <v>63741</v>
+      </c>
+      <c r="G55">
+        <v>3904</v>
+      </c>
+      <c r="H55">
+        <v>45522</v>
+      </c>
+      <c r="I55">
+        <v>382</v>
+      </c>
+      <c r="J55">
+        <v>169873</v>
+      </c>
+      <c r="K55">
+        <v>12499</v>
+      </c>
+      <c r="L55">
+        <v>182869</v>
+      </c>
+      <c r="M55">
+        <v>97006</v>
+      </c>
+      <c r="N55">
+        <v>27190</v>
+      </c>
+      <c r="O55">
+        <v>130433</v>
+      </c>
+      <c r="P55">
+        <v>45785</v>
+      </c>
+      <c r="Q55">
+        <v>206313</v>
+      </c>
+      <c r="R55">
+        <v>61900</v>
+      </c>
+      <c r="S55">
+        <v>5730</v>
+      </c>
+      <c r="T55">
+        <v>132769</v>
+      </c>
+      <c r="U55">
+        <v>363470</v>
+      </c>
+      <c r="V55">
+        <v>1706</v>
+      </c>
+      <c r="W55">
+        <v>3682</v>
+      </c>
+      <c r="X55">
+        <v>342</v>
+      </c>
+      <c r="Y55">
+        <v>1097</v>
+      </c>
+      <c r="Z55">
+        <v>123834</v>
+      </c>
+      <c r="AA55">
+        <v>6106</v>
+      </c>
+      <c r="AB55">
+        <v>66142</v>
+      </c>
+      <c r="AC55">
+        <v>303935</v>
+      </c>
+      <c r="AD55">
+        <v>1855</v>
+      </c>
+      <c r="AE55">
+        <v>409615</v>
+      </c>
+      <c r="AF55">
+        <v>23388</v>
+      </c>
+      <c r="AG55">
+        <v>18737</v>
+      </c>
+      <c r="AH55">
+        <v>229621</v>
+      </c>
+      <c r="AI55">
+        <v>20969</v>
+      </c>
+      <c r="AJ55">
+        <v>138824</v>
+      </c>
+      <c r="AK55">
+        <v>3275853</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2">
+        <v>43976</v>
+      </c>
+      <c r="B56">
+        <v>6677</v>
+      </c>
+      <c r="C56">
+        <v>314566</v>
+      </c>
+      <c r="D56">
+        <v>5997</v>
+      </c>
+      <c r="E56">
+        <v>70029</v>
+      </c>
+      <c r="F56">
+        <v>63741</v>
+      </c>
+      <c r="G56">
+        <v>4089</v>
+      </c>
+      <c r="H56">
+        <v>45522</v>
+      </c>
+      <c r="I56">
+        <v>382</v>
+      </c>
+      <c r="J56">
+        <v>174469</v>
+      </c>
+      <c r="K56">
+        <v>12860</v>
+      </c>
+      <c r="L56">
+        <v>186361</v>
+      </c>
+      <c r="M56">
+        <v>99987</v>
+      </c>
+      <c r="N56">
+        <v>27190</v>
+      </c>
+      <c r="O56">
+        <v>134188</v>
+      </c>
+      <c r="P56">
+        <v>50709</v>
+      </c>
+      <c r="Q56">
+        <v>219894</v>
+      </c>
+      <c r="R56">
+        <v>63009</v>
+      </c>
+      <c r="S56">
+        <v>5896</v>
+      </c>
+      <c r="T56">
+        <v>138584</v>
+      </c>
+      <c r="U56">
+        <v>379185</v>
+      </c>
+      <c r="V56">
+        <v>1706</v>
+      </c>
+      <c r="W56">
+        <v>3682</v>
+      </c>
+      <c r="X56">
+        <v>359</v>
+      </c>
+      <c r="Y56">
+        <v>1366</v>
+      </c>
+      <c r="Z56">
+        <v>127776</v>
+      </c>
+      <c r="AA56">
+        <v>6606</v>
+      </c>
+      <c r="AB56">
+        <v>66142</v>
+      </c>
+      <c r="AC56">
+        <v>327836</v>
+      </c>
+      <c r="AD56">
+        <v>2103</v>
+      </c>
+      <c r="AE56">
+        <v>421450</v>
+      </c>
+      <c r="AF56">
+        <v>23388</v>
+      </c>
+      <c r="AG56">
+        <v>20871</v>
+      </c>
+      <c r="AH56">
+        <v>235622</v>
+      </c>
+      <c r="AI56">
+        <v>22117</v>
+      </c>
+      <c r="AJ56">
+        <v>148049</v>
+      </c>
+      <c r="AK56">
+        <v>3412408</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B57">
+        <v>6677</v>
+      </c>
+      <c r="C57">
+        <v>322714</v>
+      </c>
+      <c r="D57">
+        <v>6319</v>
+      </c>
+      <c r="E57">
+        <v>72654</v>
+      </c>
+      <c r="F57">
+        <v>63741</v>
+      </c>
+      <c r="G57">
+        <v>4207</v>
+      </c>
+      <c r="H57">
+        <v>57479</v>
+      </c>
+      <c r="I57">
+        <v>10388</v>
+      </c>
+      <c r="J57">
+        <v>178579</v>
+      </c>
+      <c r="K57">
+        <v>13303</v>
+      </c>
+      <c r="L57">
+        <v>189313</v>
+      </c>
+      <c r="M57">
+        <v>102018</v>
+      </c>
+      <c r="N57">
+        <v>29379</v>
+      </c>
+      <c r="O57">
+        <v>140962</v>
+      </c>
+      <c r="P57">
+        <v>53309</v>
+      </c>
+      <c r="Q57">
+        <v>228914</v>
+      </c>
+      <c r="R57">
+        <v>65303</v>
+      </c>
+      <c r="S57">
+        <v>5896</v>
+      </c>
+      <c r="T57">
+        <v>141508</v>
+      </c>
+      <c r="U57">
+        <v>390757</v>
+      </c>
+      <c r="V57">
+        <v>6233</v>
+      </c>
+      <c r="W57">
+        <v>3682</v>
+      </c>
+      <c r="X57">
+        <v>438</v>
+      </c>
+      <c r="Y57">
+        <v>1366</v>
+      </c>
+      <c r="Z57">
+        <v>131595</v>
+      </c>
+      <c r="AA57">
+        <v>6677</v>
+      </c>
+      <c r="AB57">
+        <v>69818</v>
+      </c>
+      <c r="AC57">
+        <v>337159</v>
+      </c>
+      <c r="AD57">
+        <v>2255</v>
+      </c>
+      <c r="AE57">
+        <v>431739</v>
+      </c>
+      <c r="AF57">
+        <v>23388</v>
+      </c>
+      <c r="AG57">
+        <v>22049</v>
+      </c>
+      <c r="AH57">
+        <v>240588</v>
+      </c>
+      <c r="AI57">
+        <v>23076</v>
+      </c>
+      <c r="AJ57">
+        <v>157277</v>
+      </c>
+      <c r="AK57">
+        <v>3540760</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B58">
+        <v>6677</v>
+      </c>
+      <c r="C58">
+        <v>332378</v>
+      </c>
+      <c r="D58">
+        <v>6436</v>
+      </c>
+      <c r="E58">
+        <v>72654</v>
+      </c>
+      <c r="F58">
+        <v>68262</v>
+      </c>
+      <c r="G58">
+        <v>4332</v>
+      </c>
+      <c r="H58">
+        <v>59320</v>
+      </c>
+      <c r="I58">
+        <v>10872</v>
+      </c>
+      <c r="J58">
+        <v>184362</v>
+      </c>
+      <c r="K58">
+        <v>13911</v>
+      </c>
+      <c r="L58">
+        <v>193863</v>
+      </c>
+      <c r="M58">
+        <v>104747</v>
+      </c>
+      <c r="N58">
+        <v>30852</v>
+      </c>
+      <c r="O58">
+        <v>145162</v>
+      </c>
+      <c r="P58">
+        <v>55427</v>
+      </c>
+      <c r="Q58">
+        <v>241608</v>
+      </c>
+      <c r="R58">
+        <v>67961</v>
+      </c>
+      <c r="S58">
+        <v>5896</v>
+      </c>
+      <c r="T58">
+        <v>146144</v>
+      </c>
+      <c r="U58">
+        <v>405020</v>
+      </c>
+      <c r="V58">
+        <v>6836</v>
+      </c>
+      <c r="W58">
+        <v>3682</v>
+      </c>
+      <c r="X58">
+        <v>438</v>
+      </c>
+      <c r="Y58">
+        <v>1554</v>
+      </c>
+      <c r="Z58">
+        <v>136274</v>
+      </c>
+      <c r="AA58">
+        <v>6808</v>
+      </c>
+      <c r="AB58">
+        <v>72468</v>
+      </c>
+      <c r="AC58">
+        <v>350600</v>
+      </c>
+      <c r="AD58">
+        <v>2417</v>
+      </c>
+      <c r="AE58">
+        <v>442970</v>
+      </c>
+      <c r="AF58">
+        <v>23388</v>
+      </c>
+      <c r="AG58">
+        <v>23264</v>
+      </c>
+      <c r="AH58">
+        <v>240588</v>
+      </c>
+      <c r="AI58">
+        <v>23975</v>
+      </c>
+      <c r="AJ58">
+        <v>166513</v>
+      </c>
+      <c r="AK58">
+        <v>3657659</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B59">
+        <v>6677</v>
+      </c>
+      <c r="C59">
+        <v>342236</v>
+      </c>
+      <c r="D59">
+        <v>6436</v>
+      </c>
+      <c r="E59">
+        <v>72654</v>
+      </c>
+      <c r="F59">
+        <v>70275</v>
+      </c>
+      <c r="G59">
+        <v>4467</v>
+      </c>
+      <c r="H59">
+        <v>61771</v>
+      </c>
+      <c r="I59">
+        <v>11177</v>
+      </c>
+      <c r="J59">
+        <v>191977</v>
+      </c>
+      <c r="K59">
+        <v>14782</v>
+      </c>
+      <c r="L59">
+        <v>198048</v>
+      </c>
+      <c r="M59">
+        <v>108031</v>
+      </c>
+      <c r="N59">
+        <v>32449</v>
+      </c>
+      <c r="O59">
+        <v>153522</v>
+      </c>
+      <c r="P59">
+        <v>57250</v>
+      </c>
+      <c r="Q59">
+        <v>252078</v>
+      </c>
+      <c r="R59">
+        <v>70622</v>
+      </c>
+      <c r="S59">
+        <v>5896</v>
+      </c>
+      <c r="T59">
+        <v>151182</v>
+      </c>
+      <c r="U59">
+        <v>420473</v>
+      </c>
+      <c r="V59">
+        <v>7758</v>
+      </c>
+      <c r="W59">
+        <v>3682</v>
+      </c>
+      <c r="X59">
+        <v>516</v>
+      </c>
+      <c r="Y59">
+        <v>1554</v>
+      </c>
+      <c r="Z59">
+        <v>139311</v>
+      </c>
+      <c r="AA59">
+        <v>6917</v>
+      </c>
+      <c r="AB59">
+        <v>72468</v>
+      </c>
+      <c r="AC59">
+        <v>365556</v>
+      </c>
+      <c r="AD59">
+        <v>2626</v>
+      </c>
+      <c r="AE59">
+        <v>455216</v>
+      </c>
+      <c r="AF59">
+        <v>23388</v>
+      </c>
+      <c r="AG59">
+        <v>24126</v>
+      </c>
+      <c r="AH59">
+        <v>256267</v>
+      </c>
+      <c r="AI59">
+        <v>25380</v>
+      </c>
+      <c r="AJ59">
+        <v>175769</v>
+      </c>
+      <c r="AK59">
+        <v>3792537</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B60">
+        <v>6677</v>
+      </c>
+      <c r="C60">
+        <v>353874</v>
+      </c>
+      <c r="D60">
+        <v>7488</v>
+      </c>
+      <c r="E60">
+        <v>92390</v>
+      </c>
+      <c r="F60">
+        <v>72256</v>
+      </c>
+      <c r="G60">
+        <v>4543</v>
+      </c>
+      <c r="H60">
+        <v>63992</v>
+      </c>
+      <c r="I60">
+        <v>11477</v>
+      </c>
+      <c r="J60">
+        <v>199626</v>
+      </c>
+      <c r="K60">
+        <v>16141</v>
+      </c>
+      <c r="L60">
+        <v>201481</v>
+      </c>
+      <c r="M60">
+        <v>110940</v>
+      </c>
+      <c r="N60">
+        <v>33979</v>
+      </c>
+      <c r="O60">
+        <v>158729</v>
+      </c>
+      <c r="P60">
+        <v>59452</v>
+      </c>
+      <c r="Q60">
+        <v>264489</v>
+      </c>
+      <c r="R60">
+        <v>74214</v>
+      </c>
+      <c r="S60">
+        <v>5896</v>
+      </c>
+      <c r="T60">
+        <v>155436</v>
+      </c>
+      <c r="U60">
+        <v>434565</v>
+      </c>
+      <c r="V60">
+        <v>7758</v>
+      </c>
+      <c r="W60">
+        <v>3682</v>
+      </c>
+      <c r="X60">
+        <v>529</v>
+      </c>
+      <c r="Y60">
+        <v>1997</v>
+      </c>
+      <c r="Z60">
+        <v>143570</v>
+      </c>
+      <c r="AA60">
+        <v>7043</v>
+      </c>
+      <c r="AB60">
+        <v>81021</v>
+      </c>
+      <c r="AC60">
+        <v>379315</v>
+      </c>
+      <c r="AD60">
+        <v>2759</v>
+      </c>
+      <c r="AE60">
+        <v>466550</v>
+      </c>
+      <c r="AF60">
+        <v>23388</v>
+      </c>
+      <c r="AG60">
+        <v>25403</v>
+      </c>
+      <c r="AH60">
+        <v>270920</v>
+      </c>
+      <c r="AI60">
+        <v>26951</v>
+      </c>
+      <c r="AJ60">
+        <v>185051</v>
+      </c>
+      <c r="AK60">
+        <v>3953582</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B61">
+        <v>6677</v>
+      </c>
+      <c r="C61">
+        <v>363378</v>
+      </c>
+      <c r="D61">
+        <v>8017</v>
+      </c>
+      <c r="E61">
+        <v>101257</v>
+      </c>
+      <c r="F61">
+        <v>73929</v>
+      </c>
+      <c r="G61">
+        <v>4654</v>
+      </c>
+      <c r="H61">
+        <v>66417</v>
+      </c>
+      <c r="I61">
+        <v>11477</v>
+      </c>
+      <c r="J61">
+        <v>206739</v>
+      </c>
+      <c r="K61">
+        <v>17871</v>
+      </c>
+      <c r="L61">
+        <v>205780</v>
+      </c>
+      <c r="M61">
+        <v>114683</v>
+      </c>
+      <c r="N61">
+        <v>35668</v>
+      </c>
+      <c r="O61">
+        <v>164581</v>
+      </c>
+      <c r="P61">
+        <v>62916</v>
+      </c>
+      <c r="Q61">
+        <v>280217</v>
+      </c>
+      <c r="R61">
+        <v>77257</v>
+      </c>
+      <c r="S61">
+        <v>7354</v>
+      </c>
+      <c r="T61">
+        <v>161552</v>
+      </c>
+      <c r="U61">
+        <v>448661</v>
+      </c>
+      <c r="V61">
+        <v>7758</v>
+      </c>
+      <c r="W61">
+        <v>3682</v>
+      </c>
+      <c r="X61">
+        <v>686</v>
+      </c>
+      <c r="Y61">
+        <v>2210</v>
+      </c>
+      <c r="Z61">
+        <v>147490</v>
+      </c>
+      <c r="AA61">
+        <v>7164</v>
+      </c>
+      <c r="AB61">
+        <v>84497</v>
+      </c>
+      <c r="AC61">
+        <v>395490</v>
+      </c>
+      <c r="AD61">
+        <v>2829</v>
+      </c>
+      <c r="AE61">
+        <v>479155</v>
+      </c>
+      <c r="AF61">
+        <v>23388</v>
+      </c>
+      <c r="AG61">
+        <v>26376</v>
+      </c>
+      <c r="AH61">
+        <v>279288</v>
+      </c>
+      <c r="AI61">
+        <v>28433</v>
+      </c>
+      <c r="AJ61">
+        <v>194397</v>
+      </c>
+      <c r="AK61">
+        <v>4101928</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B62">
+        <v>6677</v>
+      </c>
+      <c r="C62">
+        <v>372748</v>
+      </c>
+      <c r="D62">
+        <v>8017</v>
+      </c>
+      <c r="E62">
+        <v>109097</v>
+      </c>
+      <c r="F62">
+        <v>75737</v>
+      </c>
+      <c r="G62">
+        <v>4785</v>
+      </c>
+      <c r="H62">
+        <v>69152</v>
+      </c>
+      <c r="I62">
+        <v>11477</v>
+      </c>
+      <c r="J62">
+        <v>212784</v>
+      </c>
+      <c r="K62">
+        <v>19491</v>
+      </c>
+      <c r="L62">
+        <v>205780</v>
+      </c>
+      <c r="M62">
+        <v>118138</v>
+      </c>
+      <c r="N62">
+        <v>37168</v>
+      </c>
+      <c r="O62">
+        <v>171045</v>
+      </c>
+      <c r="P62">
+        <v>65886</v>
+      </c>
+      <c r="Q62">
+        <v>293575</v>
+      </c>
+      <c r="R62">
+        <v>77508</v>
+      </c>
+      <c r="S62">
+        <v>7354</v>
+      </c>
+      <c r="T62">
+        <v>167808</v>
+      </c>
+      <c r="U62">
+        <v>463177</v>
+      </c>
+      <c r="V62">
+        <v>7758</v>
+      </c>
+      <c r="W62">
+        <v>7781</v>
+      </c>
+      <c r="X62">
+        <v>777</v>
+      </c>
+      <c r="Y62">
+        <v>2576</v>
+      </c>
+      <c r="Z62">
+        <v>152131</v>
+      </c>
+      <c r="AA62">
+        <v>7255</v>
+      </c>
+      <c r="AB62">
+        <v>87852</v>
+      </c>
+      <c r="AC62">
+        <v>409777</v>
+      </c>
+      <c r="AD62">
+        <v>2925</v>
+      </c>
+      <c r="AE62">
+        <v>491962</v>
+      </c>
+      <c r="AF62">
+        <v>23388</v>
+      </c>
+      <c r="AG62">
+        <v>27475</v>
+      </c>
+      <c r="AH62">
+        <v>289892</v>
+      </c>
+      <c r="AI62">
+        <v>30438</v>
+      </c>
+      <c r="AJ62">
+        <v>203751</v>
+      </c>
+      <c r="AK62">
+        <v>4243142</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B63">
+        <v>6677</v>
+      </c>
+      <c r="C63">
+        <v>383315</v>
+      </c>
+      <c r="D63">
+        <v>8768</v>
+      </c>
+      <c r="E63">
+        <v>109097</v>
+      </c>
+      <c r="F63">
+        <v>78090</v>
+      </c>
+      <c r="G63">
+        <v>4816</v>
+      </c>
+      <c r="H63">
+        <v>74696</v>
+      </c>
+      <c r="I63">
+        <v>11693</v>
+      </c>
+      <c r="J63">
+        <v>217537</v>
+      </c>
+      <c r="K63">
+        <v>20780</v>
+      </c>
+      <c r="L63">
+        <v>216258</v>
+      </c>
+      <c r="M63">
+        <v>121779</v>
+      </c>
+      <c r="N63">
+        <v>37897</v>
+      </c>
+      <c r="O63">
+        <v>176309</v>
+      </c>
+      <c r="P63">
+        <v>69187</v>
+      </c>
+      <c r="Q63">
+        <v>304816</v>
+      </c>
+      <c r="R63">
+        <v>82449</v>
+      </c>
+      <c r="S63">
+        <v>7354</v>
+      </c>
+      <c r="T63">
+        <v>172019</v>
+      </c>
+      <c r="U63">
+        <v>472344</v>
+      </c>
+      <c r="V63">
+        <v>7758</v>
+      </c>
+      <c r="W63">
+        <v>8127</v>
+      </c>
+      <c r="X63">
+        <v>896</v>
+      </c>
+      <c r="Y63">
+        <v>2870</v>
+      </c>
+      <c r="Z63">
+        <v>155690</v>
+      </c>
+      <c r="AA63">
+        <v>7255</v>
+      </c>
+      <c r="AB63">
+        <v>91113</v>
+      </c>
+      <c r="AC63">
+        <v>425184</v>
+      </c>
+      <c r="AD63">
+        <v>3525</v>
+      </c>
+      <c r="AE63">
+        <v>503339</v>
+      </c>
+      <c r="AF63">
+        <v>23388</v>
+      </c>
+      <c r="AG63">
+        <v>28360</v>
+      </c>
+      <c r="AH63">
+        <v>297903</v>
+      </c>
+      <c r="AI63">
+        <v>31703</v>
+      </c>
+      <c r="AJ63">
+        <v>213231</v>
+      </c>
+      <c r="AK63">
+        <v>4376223</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B64">
+        <v>6677</v>
+      </c>
+      <c r="C64">
+        <v>395681</v>
+      </c>
+      <c r="D64">
+        <v>9079</v>
+      </c>
+      <c r="E64">
+        <v>120375</v>
+      </c>
+      <c r="F64">
+        <v>81413</v>
+      </c>
+      <c r="G64">
+        <v>4902</v>
+      </c>
+      <c r="H64">
+        <v>77168</v>
+      </c>
+      <c r="I64">
+        <v>11693</v>
+      </c>
+      <c r="J64">
+        <v>223607</v>
+      </c>
+      <c r="K64">
+        <v>22378</v>
+      </c>
+      <c r="L64">
+        <v>221610</v>
+      </c>
+      <c r="M64">
+        <v>124564</v>
+      </c>
+      <c r="N64">
+        <v>39620</v>
+      </c>
+      <c r="O64">
+        <v>183067</v>
+      </c>
+      <c r="P64">
+        <v>71296</v>
+      </c>
+      <c r="Q64">
+        <v>319628</v>
+      </c>
+      <c r="R64">
+        <v>86169</v>
+      </c>
+      <c r="S64">
+        <v>8264</v>
+      </c>
+      <c r="T64">
+        <v>177481</v>
+      </c>
+      <c r="U64">
+        <v>484784</v>
+      </c>
+      <c r="V64">
+        <v>7758</v>
+      </c>
+      <c r="W64">
+        <v>8734</v>
+      </c>
+      <c r="X64">
+        <v>1012</v>
+      </c>
+      <c r="Y64">
+        <v>3257</v>
+      </c>
+      <c r="Z64">
+        <v>159567</v>
+      </c>
+      <c r="AA64">
+        <v>7255</v>
+      </c>
+      <c r="AB64">
+        <v>96329</v>
+      </c>
+      <c r="AC64">
+        <v>440789</v>
+      </c>
+      <c r="AD64">
+        <v>3788</v>
+      </c>
+      <c r="AE64">
+        <v>514433</v>
+      </c>
+      <c r="AF64">
+        <v>23388</v>
+      </c>
+      <c r="AG64">
+        <v>29066</v>
+      </c>
+      <c r="AH64">
+        <v>307621</v>
+      </c>
+      <c r="AI64">
+        <v>33081</v>
+      </c>
+      <c r="AJ64">
+        <v>222726</v>
+      </c>
+      <c r="AK64">
+        <v>4528260</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B65">
+        <v>6677</v>
+      </c>
+      <c r="C65">
+        <v>403747</v>
+      </c>
+      <c r="D65">
+        <v>9079</v>
+      </c>
+      <c r="E65">
+        <v>126726</v>
+      </c>
+      <c r="F65">
+        <v>84729</v>
+      </c>
+      <c r="G65">
+        <v>4977</v>
+      </c>
+      <c r="H65">
+        <v>80416</v>
+      </c>
+      <c r="I65">
+        <v>12064</v>
+      </c>
+      <c r="J65">
+        <v>223607</v>
+      </c>
+      <c r="K65">
+        <v>23816</v>
+      </c>
+      <c r="L65">
+        <v>227898</v>
+      </c>
+      <c r="M65">
+        <v>127895</v>
+      </c>
+      <c r="N65">
+        <v>41351</v>
+      </c>
+      <c r="O65">
+        <v>189364</v>
+      </c>
+      <c r="P65">
+        <v>74499</v>
+      </c>
+      <c r="Q65">
+        <v>334825</v>
+      </c>
+      <c r="R65">
+        <v>95348</v>
+      </c>
+      <c r="S65">
+        <v>8264</v>
+      </c>
+      <c r="T65">
+        <v>183662</v>
+      </c>
+      <c r="U65">
+        <v>498577</v>
+      </c>
+      <c r="V65">
+        <v>12454</v>
+      </c>
+      <c r="W65">
+        <v>9025</v>
+      </c>
+      <c r="X65">
+        <v>1095</v>
+      </c>
+      <c r="Y65">
+        <v>3414</v>
+      </c>
+      <c r="Z65">
+        <v>162891</v>
+      </c>
+      <c r="AA65">
+        <v>7255</v>
+      </c>
+      <c r="AB65">
+        <v>101036</v>
+      </c>
+      <c r="AC65">
+        <v>454788</v>
+      </c>
+      <c r="AD65">
+        <v>4102</v>
+      </c>
+      <c r="AE65">
+        <v>528534</v>
+      </c>
+      <c r="AF65">
+        <v>23388</v>
+      </c>
+      <c r="AG65">
+        <v>29066</v>
+      </c>
+      <c r="AH65">
+        <v>317780</v>
+      </c>
+      <c r="AI65">
+        <v>34413</v>
+      </c>
+      <c r="AJ65">
+        <v>232225</v>
+      </c>
+      <c r="AK65">
+        <v>4678987</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B66">
+        <v>6677</v>
+      </c>
+      <c r="C66">
+        <v>413733</v>
+      </c>
+      <c r="D66">
+        <v>10025</v>
+      </c>
+      <c r="E66">
+        <v>133029</v>
+      </c>
+      <c r="F66">
+        <v>88313</v>
+      </c>
+      <c r="G66">
+        <v>5059</v>
+      </c>
+      <c r="H66">
+        <v>82941</v>
+      </c>
+      <c r="I66">
+        <v>12375</v>
+      </c>
+      <c r="J66">
+        <v>223607</v>
+      </c>
+      <c r="K66">
+        <v>25300</v>
+      </c>
+      <c r="L66">
+        <v>233921</v>
+      </c>
+      <c r="M66">
+        <v>132575</v>
+      </c>
+      <c r="N66">
+        <v>42703</v>
+      </c>
+      <c r="O66">
+        <v>195677</v>
+      </c>
+      <c r="P66">
+        <v>77641</v>
+      </c>
+      <c r="Q66">
+        <v>347093</v>
+      </c>
+      <c r="R66">
+        <v>99692</v>
+      </c>
+      <c r="S66">
+        <v>8264</v>
+      </c>
+      <c r="T66">
+        <v>189252</v>
+      </c>
+      <c r="U66">
+        <v>511136</v>
+      </c>
+      <c r="V66">
+        <v>12454</v>
+      </c>
+      <c r="W66">
+        <v>9395</v>
+      </c>
+      <c r="X66">
+        <v>1346</v>
+      </c>
+      <c r="Y66">
+        <v>3739</v>
+      </c>
+      <c r="Z66">
+        <v>165824</v>
+      </c>
+      <c r="AA66">
+        <v>7255</v>
+      </c>
+      <c r="AB66">
+        <v>106933</v>
+      </c>
+      <c r="AC66">
+        <v>467129</v>
+      </c>
+      <c r="AD66">
+        <v>4358</v>
+      </c>
+      <c r="AE66">
+        <v>544981</v>
+      </c>
+      <c r="AF66">
+        <v>23388</v>
+      </c>
+      <c r="AG66">
+        <v>31138</v>
+      </c>
+      <c r="AH66">
+        <v>330663</v>
+      </c>
+      <c r="AI66">
+        <v>35117</v>
+      </c>
+      <c r="AJ66">
+        <v>241831</v>
+      </c>
+      <c r="AK66">
+        <v>4824564</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B67">
+        <v>6677</v>
+      </c>
+      <c r="C67">
+        <v>423564</v>
+      </c>
+      <c r="D67">
+        <v>10025</v>
+      </c>
+      <c r="E67">
+        <v>133029</v>
+      </c>
+      <c r="F67">
+        <v>91903</v>
+      </c>
+      <c r="G67">
+        <v>5121</v>
+      </c>
+      <c r="H67">
+        <v>85743</v>
+      </c>
+      <c r="I67">
+        <v>13667</v>
+      </c>
+      <c r="J67">
+        <v>241693</v>
+      </c>
+      <c r="K67">
+        <v>26208</v>
+      </c>
+      <c r="L67">
+        <v>239911</v>
+      </c>
+      <c r="M67">
+        <v>137452</v>
+      </c>
+      <c r="N67">
+        <v>43688</v>
+      </c>
+      <c r="O67">
+        <v>202257</v>
+      </c>
+      <c r="P67">
+        <v>80097</v>
+      </c>
+      <c r="Q67">
+        <v>360720</v>
+      </c>
+      <c r="R67">
+        <v>104045</v>
+      </c>
+      <c r="S67">
+        <v>9754</v>
+      </c>
+      <c r="T67">
+        <v>195249</v>
+      </c>
+      <c r="U67">
+        <v>524002</v>
+      </c>
+      <c r="V67">
+        <v>14629</v>
+      </c>
+      <c r="W67">
+        <v>9592</v>
+      </c>
+      <c r="X67">
+        <v>1687</v>
+      </c>
+      <c r="Y67">
+        <v>3974</v>
+      </c>
+      <c r="Z67">
+        <v>169010</v>
+      </c>
+      <c r="AA67">
+        <v>7963</v>
+      </c>
+      <c r="AB67">
+        <v>113542</v>
+      </c>
+      <c r="AC67">
+        <v>480910</v>
+      </c>
+      <c r="AD67">
+        <v>4761</v>
+      </c>
+      <c r="AE67">
+        <v>560673</v>
+      </c>
+      <c r="AF67">
+        <v>23388</v>
+      </c>
+      <c r="AG67">
+        <v>32300</v>
+      </c>
+      <c r="AH67">
+        <v>344717</v>
+      </c>
+      <c r="AI67">
+        <v>35967</v>
+      </c>
+      <c r="AJ67">
+        <v>251517</v>
+      </c>
+      <c r="AK67">
+        <v>4989435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 7th June 2020
</commit_message>
<xml_diff>
--- a/SupportFiles/TestDaily_Test.xlsx
+++ b/SupportFiles/TestDaily_Test.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK67"/>
+  <dimension ref="A1:AK68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7699,7 +7699,7 @@
         <v>12064</v>
       </c>
       <c r="J65">
-        <v>223607</v>
+        <v>230145</v>
       </c>
       <c r="K65">
         <v>23816</v>
@@ -7780,7 +7780,7 @@
         <v>232225</v>
       </c>
       <c r="AK65">
-        <v>4678987</v>
+        <v>4685525</v>
       </c>
     </row>
     <row r="66">
@@ -7812,7 +7812,7 @@
         <v>12375</v>
       </c>
       <c r="J66">
-        <v>223607</v>
+        <v>236506</v>
       </c>
       <c r="K66">
         <v>25300</v>
@@ -7893,7 +7893,7 @@
         <v>241831</v>
       </c>
       <c r="AK66">
-        <v>4824564</v>
+        <v>4837463</v>
       </c>
     </row>
     <row r="67">
@@ -7907,7 +7907,7 @@
         <v>423564</v>
       </c>
       <c r="D67">
-        <v>10025</v>
+        <v>10790</v>
       </c>
       <c r="E67">
         <v>133029</v>
@@ -7925,7 +7925,7 @@
         <v>13667</v>
       </c>
       <c r="J67">
-        <v>241693</v>
+        <v>236506</v>
       </c>
       <c r="K67">
         <v>26208</v>
@@ -8006,7 +8006,120 @@
         <v>251517</v>
       </c>
       <c r="AK67">
-        <v>4989435</v>
+        <v>4985013</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B68">
+        <v>6677</v>
+      </c>
+      <c r="C68">
+        <v>436335</v>
+      </c>
+      <c r="D68">
+        <v>11261</v>
+      </c>
+      <c r="E68">
+        <v>146605</v>
+      </c>
+      <c r="F68">
+        <v>95473</v>
+      </c>
+      <c r="G68">
+        <v>5237</v>
+      </c>
+      <c r="H68">
+        <v>89392</v>
+      </c>
+      <c r="I68">
+        <v>14780</v>
+      </c>
+      <c r="J68">
+        <v>246873</v>
+      </c>
+      <c r="K68">
+        <v>27402</v>
+      </c>
+      <c r="L68">
+        <v>245606</v>
+      </c>
+      <c r="M68">
+        <v>141688</v>
+      </c>
+      <c r="N68">
+        <v>44509</v>
+      </c>
+      <c r="O68">
+        <v>211880</v>
+      </c>
+      <c r="P68">
+        <v>84444</v>
+      </c>
+      <c r="Q68">
+        <v>372582</v>
+      </c>
+      <c r="R68">
+        <v>107796</v>
+      </c>
+      <c r="S68">
+        <v>10164</v>
+      </c>
+      <c r="T68">
+        <v>200913</v>
+      </c>
+      <c r="U68">
+        <v>538009</v>
+      </c>
+      <c r="V68">
+        <v>14629</v>
+      </c>
+      <c r="W68">
+        <v>10066</v>
+      </c>
+      <c r="X68">
+        <v>1991</v>
+      </c>
+      <c r="Y68">
+        <v>4061</v>
+      </c>
+      <c r="Z68">
+        <v>172598</v>
+      </c>
+      <c r="AA68">
+        <v>7963</v>
+      </c>
+      <c r="AB68">
+        <v>115974</v>
+      </c>
+      <c r="AC68">
+        <v>494480</v>
+      </c>
+      <c r="AD68">
+        <v>5005</v>
+      </c>
+      <c r="AE68">
+        <v>576695</v>
+      </c>
+      <c r="AF68">
+        <v>23388</v>
+      </c>
+      <c r="AG68">
+        <v>33331</v>
+      </c>
+      <c r="AH68">
+        <v>355085</v>
+      </c>
+      <c r="AI68">
+        <v>36638</v>
+      </c>
+      <c r="AJ68">
+        <v>261288</v>
+      </c>
+      <c r="AK68">
+        <v>5150818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated on 23rd June
Updated on 23rd June
</commit_message>
<xml_diff>
--- a/SupportFiles/TestDaily_Test.xlsx
+++ b/SupportFiles/TestDaily_Test.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK68"/>
+  <dimension ref="A1:AK84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8122,6 +8122,1814 @@
         <v>5150818</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B69">
+        <v>6677</v>
+      </c>
+      <c r="C69">
+        <v>454030</v>
+      </c>
+      <c r="D69">
+        <v>11516</v>
+      </c>
+      <c r="E69">
+        <v>153326</v>
+      </c>
+      <c r="F69">
+        <v>99108</v>
+      </c>
+      <c r="G69">
+        <v>5312</v>
+      </c>
+      <c r="H69">
+        <v>92942</v>
+      </c>
+      <c r="I69">
+        <v>15546</v>
+      </c>
+      <c r="J69">
+        <v>251915</v>
+      </c>
+      <c r="K69">
+        <v>29739</v>
+      </c>
+      <c r="L69">
+        <v>251686</v>
+      </c>
+      <c r="M69">
+        <v>145722</v>
+      </c>
+      <c r="N69">
+        <v>45888</v>
+      </c>
+      <c r="O69">
+        <v>218481</v>
+      </c>
+      <c r="P69">
+        <v>87721</v>
+      </c>
+      <c r="Q69">
+        <v>384442</v>
+      </c>
+      <c r="R69">
+        <v>111930</v>
+      </c>
+      <c r="S69">
+        <v>10164</v>
+      </c>
+      <c r="T69">
+        <v>208514</v>
+      </c>
+      <c r="U69">
+        <v>553063</v>
+      </c>
+      <c r="V69">
+        <v>17028</v>
+      </c>
+      <c r="W69">
+        <v>10066</v>
+      </c>
+      <c r="X69">
+        <v>2252</v>
+      </c>
+      <c r="Y69">
+        <v>4371</v>
+      </c>
+      <c r="Z69">
+        <v>176098</v>
+      </c>
+      <c r="AA69">
+        <v>8274</v>
+      </c>
+      <c r="AB69">
+        <v>124266</v>
+      </c>
+      <c r="AC69">
+        <v>506784</v>
+      </c>
+      <c r="AD69">
+        <v>5005</v>
+      </c>
+      <c r="AE69">
+        <v>592970</v>
+      </c>
+      <c r="AF69">
+        <v>23388</v>
+      </c>
+      <c r="AG69">
+        <v>35263</v>
+      </c>
+      <c r="AH69">
+        <v>360258</v>
+      </c>
+      <c r="AI69">
+        <v>37166</v>
+      </c>
+      <c r="AJ69">
+        <v>271074</v>
+      </c>
+      <c r="AK69">
+        <v>5311985</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B70">
+        <v>6677</v>
+      </c>
+      <c r="C70">
+        <v>468276</v>
+      </c>
+      <c r="D70">
+        <v>12012</v>
+      </c>
+      <c r="E70">
+        <v>153326</v>
+      </c>
+      <c r="F70">
+        <v>102318</v>
+      </c>
+      <c r="G70">
+        <v>5385</v>
+      </c>
+      <c r="H70">
+        <v>96963</v>
+      </c>
+      <c r="I70">
+        <v>16277</v>
+      </c>
+      <c r="J70">
+        <v>255615</v>
+      </c>
+      <c r="K70">
+        <v>31455</v>
+      </c>
+      <c r="L70">
+        <v>256289</v>
+      </c>
+      <c r="M70">
+        <v>150220</v>
+      </c>
+      <c r="N70">
+        <v>46416</v>
+      </c>
+      <c r="O70">
+        <v>227906</v>
+      </c>
+      <c r="P70">
+        <v>92325</v>
+      </c>
+      <c r="Q70">
+        <v>393221</v>
+      </c>
+      <c r="R70">
+        <v>113956</v>
+      </c>
+      <c r="S70">
+        <v>10164</v>
+      </c>
+      <c r="T70">
+        <v>215194</v>
+      </c>
+      <c r="U70">
+        <v>565290</v>
+      </c>
+      <c r="V70">
+        <v>17028</v>
+      </c>
+      <c r="W70">
+        <v>10746</v>
+      </c>
+      <c r="X70">
+        <v>2496</v>
+      </c>
+      <c r="Y70">
+        <v>4719</v>
+      </c>
+      <c r="Z70">
+        <v>179415</v>
+      </c>
+      <c r="AA70">
+        <v>8472</v>
+      </c>
+      <c r="AB70">
+        <v>129821</v>
+      </c>
+      <c r="AC70">
+        <v>518350</v>
+      </c>
+      <c r="AD70">
+        <v>5547</v>
+      </c>
+      <c r="AE70">
+        <v>607952</v>
+      </c>
+      <c r="AF70">
+        <v>23388</v>
+      </c>
+      <c r="AG70">
+        <v>37453</v>
+      </c>
+      <c r="AH70">
+        <v>380723</v>
+      </c>
+      <c r="AI70">
+        <v>39133</v>
+      </c>
+      <c r="AJ70">
+        <v>280098</v>
+      </c>
+      <c r="AK70">
+        <v>5464626</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B71">
+        <v>6677</v>
+      </c>
+      <c r="C71">
+        <v>483361</v>
+      </c>
+      <c r="D71">
+        <v>12012</v>
+      </c>
+      <c r="E71">
+        <v>153326</v>
+      </c>
+      <c r="F71">
+        <v>105588</v>
+      </c>
+      <c r="G71">
+        <v>5385</v>
+      </c>
+      <c r="H71">
+        <v>96963</v>
+      </c>
+      <c r="I71">
+        <v>16277</v>
+      </c>
+      <c r="J71">
+        <v>261079</v>
+      </c>
+      <c r="K71">
+        <v>31455</v>
+      </c>
+      <c r="L71">
+        <v>261587</v>
+      </c>
+      <c r="M71">
+        <v>153692</v>
+      </c>
+      <c r="N71">
+        <v>47655</v>
+      </c>
+      <c r="O71">
+        <v>235816</v>
+      </c>
+      <c r="P71">
+        <v>92325</v>
+      </c>
+      <c r="Q71">
+        <v>400257</v>
+      </c>
+      <c r="R71">
+        <v>126088</v>
+      </c>
+      <c r="S71">
+        <v>10249</v>
+      </c>
+      <c r="T71">
+        <v>220936</v>
+      </c>
+      <c r="U71">
+        <v>579294</v>
+      </c>
+      <c r="V71">
+        <v>18612</v>
+      </c>
+      <c r="W71">
+        <v>11247</v>
+      </c>
+      <c r="X71">
+        <v>2747</v>
+      </c>
+      <c r="Y71">
+        <v>4896</v>
+      </c>
+      <c r="Z71">
+        <v>182384</v>
+      </c>
+      <c r="AA71">
+        <v>11752</v>
+      </c>
+      <c r="AB71">
+        <v>136343</v>
+      </c>
+      <c r="AC71">
+        <v>530031</v>
+      </c>
+      <c r="AD71">
+        <v>5815</v>
+      </c>
+      <c r="AE71">
+        <v>621171</v>
+      </c>
+      <c r="AF71">
+        <v>23388</v>
+      </c>
+      <c r="AG71">
+        <v>38572</v>
+      </c>
+      <c r="AH71">
+        <v>391286</v>
+      </c>
+      <c r="AI71">
+        <v>40264</v>
+      </c>
+      <c r="AJ71">
+        <v>287900</v>
+      </c>
+      <c r="AK71">
+        <v>5606430</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B72">
+        <v>6677</v>
+      </c>
+      <c r="C72">
+        <v>498716</v>
+      </c>
+      <c r="D72">
+        <v>13035</v>
+      </c>
+      <c r="E72">
+        <v>153326</v>
+      </c>
+      <c r="F72">
+        <v>109483</v>
+      </c>
+      <c r="G72">
+        <v>5532</v>
+      </c>
+      <c r="H72">
+        <v>96963</v>
+      </c>
+      <c r="I72">
+        <v>17179</v>
+      </c>
+      <c r="J72">
+        <v>266156</v>
+      </c>
+      <c r="K72">
+        <v>35332</v>
+      </c>
+      <c r="L72">
+        <v>266404</v>
+      </c>
+      <c r="M72">
+        <v>158470</v>
+      </c>
+      <c r="N72">
+        <v>48922</v>
+      </c>
+      <c r="O72">
+        <v>241891</v>
+      </c>
+      <c r="P72">
+        <v>95500</v>
+      </c>
+      <c r="Q72">
+        <v>408506</v>
+      </c>
+      <c r="R72">
+        <v>131006</v>
+      </c>
+      <c r="S72">
+        <v>10249</v>
+      </c>
+      <c r="T72">
+        <v>228042</v>
+      </c>
+      <c r="U72">
+        <v>595282</v>
+      </c>
+      <c r="V72">
+        <v>19756</v>
+      </c>
+      <c r="W72">
+        <v>11505</v>
+      </c>
+      <c r="X72">
+        <v>2747</v>
+      </c>
+      <c r="Y72">
+        <v>5220</v>
+      </c>
+      <c r="Z72">
+        <v>185401</v>
+      </c>
+      <c r="AA72">
+        <v>11752</v>
+      </c>
+      <c r="AB72">
+        <v>144467</v>
+      </c>
+      <c r="AC72">
+        <v>543312</v>
+      </c>
+      <c r="AD72">
+        <v>6161</v>
+      </c>
+      <c r="AE72">
+        <v>638846</v>
+      </c>
+      <c r="AF72">
+        <v>23388</v>
+      </c>
+      <c r="AG72">
+        <v>40027</v>
+      </c>
+      <c r="AH72">
+        <v>404637</v>
+      </c>
+      <c r="AI72">
+        <v>40872</v>
+      </c>
+      <c r="AJ72">
+        <v>297419</v>
+      </c>
+      <c r="AK72">
+        <v>5762181</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B73">
+        <v>6677</v>
+      </c>
+      <c r="C73">
+        <v>510318</v>
+      </c>
+      <c r="D73">
+        <v>13035</v>
+      </c>
+      <c r="E73">
+        <v>181108</v>
+      </c>
+      <c r="F73">
+        <v>113225</v>
+      </c>
+      <c r="G73">
+        <v>5636</v>
+      </c>
+      <c r="H73">
+        <v>96963</v>
+      </c>
+      <c r="I73">
+        <v>17179</v>
+      </c>
+      <c r="J73">
+        <v>271516</v>
+      </c>
+      <c r="K73">
+        <v>37858</v>
+      </c>
+      <c r="L73">
+        <v>272924</v>
+      </c>
+      <c r="M73">
+        <v>162967</v>
+      </c>
+      <c r="N73">
+        <v>50222</v>
+      </c>
+      <c r="O73">
+        <v>247267</v>
+      </c>
+      <c r="P73">
+        <v>99931</v>
+      </c>
+      <c r="Q73">
+        <v>416506</v>
+      </c>
+      <c r="R73">
+        <v>135974</v>
+      </c>
+      <c r="S73">
+        <v>10855</v>
+      </c>
+      <c r="T73">
+        <v>233740</v>
+      </c>
+      <c r="U73">
+        <v>610790</v>
+      </c>
+      <c r="V73">
+        <v>20528</v>
+      </c>
+      <c r="W73">
+        <v>11889</v>
+      </c>
+      <c r="X73">
+        <v>3152</v>
+      </c>
+      <c r="Y73">
+        <v>5667</v>
+      </c>
+      <c r="Z73">
+        <v>185410</v>
+      </c>
+      <c r="AA73">
+        <v>11752</v>
+      </c>
+      <c r="AB73">
+        <v>154498</v>
+      </c>
+      <c r="AC73">
+        <v>558064</v>
+      </c>
+      <c r="AD73">
+        <v>6692</v>
+      </c>
+      <c r="AE73">
+        <v>655675</v>
+      </c>
+      <c r="AF73">
+        <v>23388</v>
+      </c>
+      <c r="AG73">
+        <v>41389</v>
+      </c>
+      <c r="AH73">
+        <v>420669</v>
+      </c>
+      <c r="AI73">
+        <v>41888</v>
+      </c>
+      <c r="AJ73">
+        <v>306941</v>
+      </c>
+      <c r="AK73">
+        <v>5942293</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B74">
+        <v>6677</v>
+      </c>
+      <c r="C74">
+        <v>522093</v>
+      </c>
+      <c r="D74">
+        <v>13035</v>
+      </c>
+      <c r="E74">
+        <v>188090</v>
+      </c>
+      <c r="F74">
+        <v>116671</v>
+      </c>
+      <c r="G74">
+        <v>5708</v>
+      </c>
+      <c r="H74">
+        <v>98603</v>
+      </c>
+      <c r="I74">
+        <v>17179</v>
+      </c>
+      <c r="J74">
+        <v>277463</v>
+      </c>
+      <c r="K74">
+        <v>39298</v>
+      </c>
+      <c r="L74">
+        <v>278137</v>
+      </c>
+      <c r="M74">
+        <v>167501</v>
+      </c>
+      <c r="N74">
+        <v>51420</v>
+      </c>
+      <c r="O74">
+        <v>254059</v>
+      </c>
+      <c r="P74">
+        <v>102092</v>
+      </c>
+      <c r="Q74">
+        <v>426341</v>
+      </c>
+      <c r="R74">
+        <v>140457</v>
+      </c>
+      <c r="S74">
+        <v>10986</v>
+      </c>
+      <c r="T74">
+        <v>241461</v>
+      </c>
+      <c r="U74">
+        <v>626521</v>
+      </c>
+      <c r="V74">
+        <v>20528</v>
+      </c>
+      <c r="W74">
+        <v>12219</v>
+      </c>
+      <c r="X74">
+        <v>3152</v>
+      </c>
+      <c r="Y74">
+        <v>6104</v>
+      </c>
+      <c r="Z74">
+        <v>192576</v>
+      </c>
+      <c r="AA74">
+        <v>11752</v>
+      </c>
+      <c r="AB74">
+        <v>165548</v>
+      </c>
+      <c r="AC74">
+        <v>571543</v>
+      </c>
+      <c r="AD74">
+        <v>6692</v>
+      </c>
+      <c r="AE74">
+        <v>673906</v>
+      </c>
+      <c r="AF74">
+        <v>23388</v>
+      </c>
+      <c r="AG74">
+        <v>41389</v>
+      </c>
+      <c r="AH74">
+        <v>435601</v>
+      </c>
+      <c r="AI74">
+        <v>42783</v>
+      </c>
+      <c r="AJ74">
+        <v>315699</v>
+      </c>
+      <c r="AK74">
+        <v>6106672</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B75">
+        <v>6677</v>
+      </c>
+      <c r="C75">
+        <v>536570</v>
+      </c>
+      <c r="D75">
+        <v>14518</v>
+      </c>
+      <c r="E75">
+        <v>188090</v>
+      </c>
+      <c r="F75">
+        <v>120086</v>
+      </c>
+      <c r="G75">
+        <v>5839</v>
+      </c>
+      <c r="H75">
+        <v>101554</v>
+      </c>
+      <c r="I75">
+        <v>17179</v>
+      </c>
+      <c r="J75">
+        <v>283239</v>
+      </c>
+      <c r="K75">
+        <v>40723</v>
+      </c>
+      <c r="L75">
+        <v>283623</v>
+      </c>
+      <c r="M75">
+        <v>171560</v>
+      </c>
+      <c r="N75">
+        <v>52737</v>
+      </c>
+      <c r="O75">
+        <v>254059</v>
+      </c>
+      <c r="P75">
+        <v>102092</v>
+      </c>
+      <c r="Q75">
+        <v>436518</v>
+      </c>
+      <c r="R75">
+        <v>144842</v>
+      </c>
+      <c r="S75">
+        <v>11135</v>
+      </c>
+      <c r="T75">
+        <v>246973</v>
+      </c>
+      <c r="U75">
+        <v>643057</v>
+      </c>
+      <c r="V75">
+        <v>24046</v>
+      </c>
+      <c r="W75">
+        <v>12560</v>
+      </c>
+      <c r="X75">
+        <v>3727</v>
+      </c>
+      <c r="Y75">
+        <v>6466</v>
+      </c>
+      <c r="Z75">
+        <v>196456</v>
+      </c>
+      <c r="AA75">
+        <v>11752</v>
+      </c>
+      <c r="AB75">
+        <v>176533</v>
+      </c>
+      <c r="AC75">
+        <v>584954</v>
+      </c>
+      <c r="AD75">
+        <v>6692</v>
+      </c>
+      <c r="AE75">
+        <v>691817</v>
+      </c>
+      <c r="AF75">
+        <v>23388</v>
+      </c>
+      <c r="AG75">
+        <v>43972</v>
+      </c>
+      <c r="AH75">
+        <v>435601</v>
+      </c>
+      <c r="AI75">
+        <v>44040</v>
+      </c>
+      <c r="AJ75">
+        <v>324707</v>
+      </c>
+      <c r="AK75">
+        <v>6247782</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B76">
+        <v>6677</v>
+      </c>
+      <c r="C76">
+        <v>552202</v>
+      </c>
+      <c r="D76">
+        <v>14518</v>
+      </c>
+      <c r="E76">
+        <v>188090</v>
+      </c>
+      <c r="F76">
+        <v>123629</v>
+      </c>
+      <c r="G76">
+        <v>5937</v>
+      </c>
+      <c r="H76">
+        <v>103895</v>
+      </c>
+      <c r="I76">
+        <v>18445</v>
+      </c>
+      <c r="J76">
+        <v>290592</v>
+      </c>
+      <c r="K76">
+        <v>41835</v>
+      </c>
+      <c r="L76">
+        <v>288565</v>
+      </c>
+      <c r="M76">
+        <v>185722</v>
+      </c>
+      <c r="N76">
+        <v>53946</v>
+      </c>
+      <c r="O76">
+        <v>266163</v>
+      </c>
+      <c r="P76">
+        <v>102092</v>
+      </c>
+      <c r="Q76">
+        <v>443969</v>
+      </c>
+      <c r="R76">
+        <v>149164</v>
+      </c>
+      <c r="S76">
+        <v>11135</v>
+      </c>
+      <c r="T76">
+        <v>252762</v>
+      </c>
+      <c r="U76">
+        <v>659481</v>
+      </c>
+      <c r="V76">
+        <v>25226</v>
+      </c>
+      <c r="W76">
+        <v>12560</v>
+      </c>
+      <c r="X76">
+        <v>4327</v>
+      </c>
+      <c r="Y76">
+        <v>6478</v>
+      </c>
+      <c r="Z76">
+        <v>200014</v>
+      </c>
+      <c r="AA76">
+        <v>11752</v>
+      </c>
+      <c r="AB76">
+        <v>182225</v>
+      </c>
+      <c r="AC76">
+        <v>598920</v>
+      </c>
+      <c r="AD76">
+        <v>6692</v>
+      </c>
+      <c r="AE76">
+        <v>710599</v>
+      </c>
+      <c r="AF76">
+        <v>23388</v>
+      </c>
+      <c r="AG76">
+        <v>46015</v>
+      </c>
+      <c r="AH76">
+        <v>467702</v>
+      </c>
+      <c r="AI76">
+        <v>45344</v>
+      </c>
+      <c r="AJ76">
+        <v>333733</v>
+      </c>
+      <c r="AK76">
+        <v>6433794</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B77">
+        <v>6677</v>
+      </c>
+      <c r="C77">
+        <v>567375</v>
+      </c>
+      <c r="D77">
+        <v>15453</v>
+      </c>
+      <c r="E77">
+        <v>217088</v>
+      </c>
+      <c r="F77">
+        <v>127126</v>
+      </c>
+      <c r="G77">
+        <v>6027</v>
+      </c>
+      <c r="H77">
+        <v>107172</v>
+      </c>
+      <c r="I77">
+        <v>18445</v>
+      </c>
+      <c r="J77">
+        <v>296697</v>
+      </c>
+      <c r="K77">
+        <v>42703</v>
+      </c>
+      <c r="L77">
+        <v>292909</v>
+      </c>
+      <c r="M77">
+        <v>189914</v>
+      </c>
+      <c r="N77">
+        <v>54484</v>
+      </c>
+      <c r="O77">
+        <v>271416</v>
+      </c>
+      <c r="P77">
+        <v>108576</v>
+      </c>
+      <c r="Q77">
+        <v>449331</v>
+      </c>
+      <c r="R77">
+        <v>151686</v>
+      </c>
+      <c r="S77">
+        <v>11260</v>
+      </c>
+      <c r="T77">
+        <v>258040</v>
+      </c>
+      <c r="U77">
+        <v>671348</v>
+      </c>
+      <c r="V77">
+        <v>26458</v>
+      </c>
+      <c r="W77">
+        <v>13353</v>
+      </c>
+      <c r="X77">
+        <v>4919</v>
+      </c>
+      <c r="Y77">
+        <v>7132</v>
+      </c>
+      <c r="Z77">
+        <v>202513</v>
+      </c>
+      <c r="AA77">
+        <v>11752</v>
+      </c>
+      <c r="AB77">
+        <v>188699</v>
+      </c>
+      <c r="AC77">
+        <v>609296</v>
+      </c>
+      <c r="AD77">
+        <v>6692</v>
+      </c>
+      <c r="AE77">
+        <v>729002</v>
+      </c>
+      <c r="AF77">
+        <v>23388</v>
+      </c>
+      <c r="AG77">
+        <v>47683</v>
+      </c>
+      <c r="AH77">
+        <v>467702</v>
+      </c>
+      <c r="AI77">
+        <v>46573</v>
+      </c>
+      <c r="AJ77">
+        <v>343242</v>
+      </c>
+      <c r="AK77">
+        <v>6592131</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B78">
+        <v>6677</v>
+      </c>
+      <c r="C78">
+        <v>583286</v>
+      </c>
+      <c r="D78">
+        <v>16158</v>
+      </c>
+      <c r="E78">
+        <v>227109</v>
+      </c>
+      <c r="F78">
+        <v>130783</v>
+      </c>
+      <c r="G78">
+        <v>6115</v>
+      </c>
+      <c r="H78">
+        <v>110062</v>
+      </c>
+      <c r="I78">
+        <v>19090</v>
+      </c>
+      <c r="J78">
+        <v>304483</v>
+      </c>
+      <c r="K78">
+        <v>44378</v>
+      </c>
+      <c r="L78">
+        <v>296335</v>
+      </c>
+      <c r="M78">
+        <v>193421</v>
+      </c>
+      <c r="N78">
+        <v>56106</v>
+      </c>
+      <c r="O78">
+        <v>276174</v>
+      </c>
+      <c r="P78">
+        <v>110813</v>
+      </c>
+      <c r="Q78">
+        <v>457267</v>
+      </c>
+      <c r="R78">
+        <v>157117</v>
+      </c>
+      <c r="S78">
+        <v>11537</v>
+      </c>
+      <c r="T78">
+        <v>263983</v>
+      </c>
+      <c r="U78">
+        <v>686488</v>
+      </c>
+      <c r="V78">
+        <v>26458</v>
+      </c>
+      <c r="W78">
+        <v>13878</v>
+      </c>
+      <c r="X78">
+        <v>5524</v>
+      </c>
+      <c r="Y78">
+        <v>7835</v>
+      </c>
+      <c r="Z78">
+        <v>205501</v>
+      </c>
+      <c r="AA78">
+        <v>11752</v>
+      </c>
+      <c r="AB78">
+        <v>198211</v>
+      </c>
+      <c r="AC78">
+        <v>622334</v>
+      </c>
+      <c r="AD78">
+        <v>6692</v>
+      </c>
+      <c r="AE78">
+        <v>748244</v>
+      </c>
+      <c r="AF78">
+        <v>44431</v>
+      </c>
+      <c r="AG78">
+        <v>49208</v>
+      </c>
+      <c r="AH78">
+        <v>467702</v>
+      </c>
+      <c r="AI78">
+        <v>47870</v>
+      </c>
+      <c r="AJ78">
+        <v>351754</v>
+      </c>
+      <c r="AK78">
+        <v>6764776</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B79">
+        <v>6677</v>
+      </c>
+      <c r="C79">
+        <v>598474</v>
+      </c>
+      <c r="D79">
+        <v>16630</v>
+      </c>
+      <c r="E79">
+        <v>235214</v>
+      </c>
+      <c r="F79">
+        <v>134402</v>
+      </c>
+      <c r="G79">
+        <v>6233</v>
+      </c>
+      <c r="H79">
+        <v>113613</v>
+      </c>
+      <c r="I79">
+        <v>19090</v>
+      </c>
+      <c r="J79">
+        <v>312576</v>
+      </c>
+      <c r="K79">
+        <v>45685</v>
+      </c>
+      <c r="L79">
+        <v>303671</v>
+      </c>
+      <c r="M79">
+        <v>197703</v>
+      </c>
+      <c r="N79">
+        <v>57479</v>
+      </c>
+      <c r="O79">
+        <v>282268</v>
+      </c>
+      <c r="P79">
+        <v>113004</v>
+      </c>
+      <c r="Q79">
+        <v>464798</v>
+      </c>
+      <c r="R79">
+        <v>161829</v>
+      </c>
+      <c r="S79">
+        <v>11626</v>
+      </c>
+      <c r="T79">
+        <v>271205</v>
+      </c>
+      <c r="U79">
+        <v>686488</v>
+      </c>
+      <c r="V79">
+        <v>29865</v>
+      </c>
+      <c r="W79">
+        <v>14316</v>
+      </c>
+      <c r="X79">
+        <v>6035</v>
+      </c>
+      <c r="Y79">
+        <v>8387</v>
+      </c>
+      <c r="Z79">
+        <v>208472</v>
+      </c>
+      <c r="AA79">
+        <v>11752</v>
+      </c>
+      <c r="AB79">
+        <v>208408</v>
+      </c>
+      <c r="AC79">
+        <v>637937</v>
+      </c>
+      <c r="AD79">
+        <v>6692</v>
+      </c>
+      <c r="AE79">
+        <v>773707</v>
+      </c>
+      <c r="AF79">
+        <v>45911</v>
+      </c>
+      <c r="AG79">
+        <v>50268</v>
+      </c>
+      <c r="AH79">
+        <v>496206</v>
+      </c>
+      <c r="AI79">
+        <v>49462</v>
+      </c>
+      <c r="AJ79">
+        <v>360976</v>
+      </c>
+      <c r="AK79">
+        <v>6947059</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B80">
+        <v>6677</v>
+      </c>
+      <c r="C80">
+        <v>612397</v>
+      </c>
+      <c r="D80">
+        <v>16630</v>
+      </c>
+      <c r="E80">
+        <v>246590</v>
+      </c>
+      <c r="F80">
+        <v>139584</v>
+      </c>
+      <c r="G80">
+        <v>6315</v>
+      </c>
+      <c r="H80">
+        <v>116329</v>
+      </c>
+      <c r="I80">
+        <v>19090</v>
+      </c>
+      <c r="J80">
+        <v>321302</v>
+      </c>
+      <c r="K80">
+        <v>46996</v>
+      </c>
+      <c r="L80">
+        <v>308744</v>
+      </c>
+      <c r="M80">
+        <v>202808</v>
+      </c>
+      <c r="N80">
+        <v>59214</v>
+      </c>
+      <c r="O80">
+        <v>289027</v>
+      </c>
+      <c r="P80">
+        <v>115186</v>
+      </c>
+      <c r="Q80">
+        <v>473507</v>
+      </c>
+      <c r="R80">
+        <v>169035</v>
+      </c>
+      <c r="S80">
+        <v>12082</v>
+      </c>
+      <c r="T80">
+        <v>277451</v>
+      </c>
+      <c r="U80">
+        <v>719637</v>
+      </c>
+      <c r="V80">
+        <v>30476</v>
+      </c>
+      <c r="W80">
+        <v>14647</v>
+      </c>
+      <c r="X80">
+        <v>6661</v>
+      </c>
+      <c r="Y80">
+        <v>9039</v>
+      </c>
+      <c r="Z80">
+        <v>212224</v>
+      </c>
+      <c r="AA80">
+        <v>11752</v>
+      </c>
+      <c r="AB80">
+        <v>219528</v>
+      </c>
+      <c r="AC80">
+        <v>654816</v>
+      </c>
+      <c r="AD80">
+        <v>6692</v>
+      </c>
+      <c r="AE80">
+        <v>800443</v>
+      </c>
+      <c r="AF80">
+        <v>45911</v>
+      </c>
+      <c r="AG80">
+        <v>51495</v>
+      </c>
+      <c r="AH80">
+        <v>515280</v>
+      </c>
+      <c r="AI80">
+        <v>50796</v>
+      </c>
+      <c r="AJ80">
+        <v>370291</v>
+      </c>
+      <c r="AK80">
+        <v>7158652</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B81">
+        <v>6677</v>
+      </c>
+      <c r="C81">
+        <v>630006</v>
+      </c>
+      <c r="D81">
+        <v>18008</v>
+      </c>
+      <c r="E81">
+        <v>258797</v>
+      </c>
+      <c r="F81">
+        <v>145562</v>
+      </c>
+      <c r="G81">
+        <v>6438</v>
+      </c>
+      <c r="H81">
+        <v>120523</v>
+      </c>
+      <c r="I81">
+        <v>19090</v>
+      </c>
+      <c r="J81">
+        <v>334376</v>
+      </c>
+      <c r="K81">
+        <v>49718</v>
+      </c>
+      <c r="L81">
+        <v>314301</v>
+      </c>
+      <c r="M81">
+        <v>207675</v>
+      </c>
+      <c r="N81">
+        <v>60814</v>
+      </c>
+      <c r="O81">
+        <v>295202</v>
+      </c>
+      <c r="P81">
+        <v>117569</v>
+      </c>
+      <c r="Q81">
+        <v>484060</v>
+      </c>
+      <c r="R81">
+        <v>173729</v>
+      </c>
+      <c r="S81">
+        <v>12516</v>
+      </c>
+      <c r="T81">
+        <v>282674</v>
+      </c>
+      <c r="U81">
+        <v>737597</v>
+      </c>
+      <c r="V81">
+        <v>32093</v>
+      </c>
+      <c r="W81">
+        <v>15104</v>
+      </c>
+      <c r="X81">
+        <v>7496</v>
+      </c>
+      <c r="Y81">
+        <v>10102</v>
+      </c>
+      <c r="Z81">
+        <v>216607</v>
+      </c>
+      <c r="AA81">
+        <v>11992</v>
+      </c>
+      <c r="AB81">
+        <v>227012</v>
+      </c>
+      <c r="AC81">
+        <v>667643</v>
+      </c>
+      <c r="AD81">
+        <v>6882</v>
+      </c>
+      <c r="AE81">
+        <v>827980</v>
+      </c>
+      <c r="AF81">
+        <v>50569</v>
+      </c>
+      <c r="AG81">
+        <v>52752</v>
+      </c>
+      <c r="AH81">
+        <v>532505</v>
+      </c>
+      <c r="AI81">
+        <v>53155</v>
+      </c>
+      <c r="AJ81">
+        <v>380612</v>
+      </c>
+      <c r="AK81">
+        <v>7367836</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B82">
+        <v>6677</v>
+      </c>
+      <c r="C82">
+        <v>652377</v>
+      </c>
+      <c r="D82">
+        <v>18008</v>
+      </c>
+      <c r="E82">
+        <v>273047</v>
+      </c>
+      <c r="F82">
+        <v>151148</v>
+      </c>
+      <c r="G82">
+        <v>6578</v>
+      </c>
+      <c r="H82">
+        <v>123983</v>
+      </c>
+      <c r="I82">
+        <v>19090</v>
+      </c>
+      <c r="J82">
+        <v>351909</v>
+      </c>
+      <c r="K82">
+        <v>51404</v>
+      </c>
+      <c r="L82">
+        <v>319414</v>
+      </c>
+      <c r="M82">
+        <v>212430</v>
+      </c>
+      <c r="N82">
+        <v>62580</v>
+      </c>
+      <c r="O82">
+        <v>301209</v>
+      </c>
+      <c r="P82">
+        <v>120892</v>
+      </c>
+      <c r="Q82">
+        <v>493893</v>
+      </c>
+      <c r="R82">
+        <v>178559</v>
+      </c>
+      <c r="S82">
+        <v>12629</v>
+      </c>
+      <c r="T82">
+        <v>290831</v>
+      </c>
+      <c r="U82">
+        <v>756809</v>
+      </c>
+      <c r="V82">
+        <v>32093</v>
+      </c>
+      <c r="W82">
+        <v>15346</v>
+      </c>
+      <c r="X82">
+        <v>8284</v>
+      </c>
+      <c r="Y82">
+        <v>10102</v>
+      </c>
+      <c r="Z82">
+        <v>219774</v>
+      </c>
+      <c r="AA82">
+        <v>12409</v>
+      </c>
+      <c r="AB82">
+        <v>235700</v>
+      </c>
+      <c r="AC82">
+        <v>683017</v>
+      </c>
+      <c r="AD82">
+        <v>7183</v>
+      </c>
+      <c r="AE82">
+        <v>861211</v>
+      </c>
+      <c r="AF82">
+        <v>53757</v>
+      </c>
+      <c r="AG82">
+        <v>53905</v>
+      </c>
+      <c r="AH82">
+        <v>542972</v>
+      </c>
+      <c r="AI82">
+        <v>54512</v>
+      </c>
+      <c r="AJ82">
+        <v>390942</v>
+      </c>
+      <c r="AK82">
+        <v>7584674</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B83">
+        <v>6677</v>
+      </c>
+      <c r="C83">
+        <v>676828</v>
+      </c>
+      <c r="D83">
+        <v>18008</v>
+      </c>
+      <c r="E83">
+        <v>288306</v>
+      </c>
+      <c r="F83">
+        <v>156926</v>
+      </c>
+      <c r="G83">
+        <v>6677</v>
+      </c>
+      <c r="H83">
+        <v>126246</v>
+      </c>
+      <c r="I83">
+        <v>19090</v>
+      </c>
+      <c r="J83">
+        <v>370014</v>
+      </c>
+      <c r="K83">
+        <v>52301</v>
+      </c>
+      <c r="L83">
+        <v>324874</v>
+      </c>
+      <c r="M83">
+        <v>217797</v>
+      </c>
+      <c r="N83">
+        <v>64338</v>
+      </c>
+      <c r="O83">
+        <v>307638</v>
+      </c>
+      <c r="P83">
+        <v>121770</v>
+      </c>
+      <c r="Q83">
+        <v>506765</v>
+      </c>
+      <c r="R83">
+        <v>183201</v>
+      </c>
+      <c r="S83">
+        <v>12838</v>
+      </c>
+      <c r="T83">
+        <v>296943</v>
+      </c>
+      <c r="U83">
+        <v>775958</v>
+      </c>
+      <c r="V83">
+        <v>35943</v>
+      </c>
+      <c r="W83">
+        <v>15346</v>
+      </c>
+      <c r="X83">
+        <v>8718</v>
+      </c>
+      <c r="Y83">
+        <v>10102</v>
+      </c>
+      <c r="Z83">
+        <v>224402</v>
+      </c>
+      <c r="AA83">
+        <v>12409</v>
+      </c>
+      <c r="AB83">
+        <v>235700</v>
+      </c>
+      <c r="AC83">
+        <v>699126</v>
+      </c>
+      <c r="AD83">
+        <v>9354</v>
+      </c>
+      <c r="AE83">
+        <v>892612</v>
+      </c>
+      <c r="AF83">
+        <v>57054</v>
+      </c>
+      <c r="AG83">
+        <v>54983</v>
+      </c>
+      <c r="AH83">
+        <v>542972</v>
+      </c>
+      <c r="AI83">
+        <v>55819</v>
+      </c>
+      <c r="AJ83">
+        <v>401491</v>
+      </c>
+      <c r="AK83">
+        <v>7789226</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B84">
+        <v>6677</v>
+      </c>
+      <c r="C84">
+        <v>693548</v>
+      </c>
+      <c r="D84">
+        <v>19799</v>
+      </c>
+      <c r="E84">
+        <v>301557</v>
+      </c>
+      <c r="F84">
+        <v>163476</v>
+      </c>
+      <c r="G84">
+        <v>6745</v>
+      </c>
+      <c r="H84">
+        <v>129731</v>
+      </c>
+      <c r="I84">
+        <v>19090</v>
+      </c>
+      <c r="J84">
+        <v>384696</v>
+      </c>
+      <c r="K84">
+        <v>53050</v>
+      </c>
+      <c r="L84">
+        <v>329343</v>
+      </c>
+      <c r="M84">
+        <v>222948</v>
+      </c>
+      <c r="N84">
+        <v>65189</v>
+      </c>
+      <c r="O84">
+        <v>313687</v>
+      </c>
+      <c r="P84">
+        <v>124008</v>
+      </c>
+      <c r="Q84">
+        <v>515969</v>
+      </c>
+      <c r="R84">
+        <v>185903</v>
+      </c>
+      <c r="S84">
+        <v>13018</v>
+      </c>
+      <c r="T84">
+        <v>302673</v>
+      </c>
+      <c r="U84">
+        <v>789016</v>
+      </c>
+      <c r="V84">
+        <v>38286</v>
+      </c>
+      <c r="W84">
+        <v>16296</v>
+      </c>
+      <c r="X84">
+        <v>9277</v>
+      </c>
+      <c r="Y84">
+        <v>10599</v>
+      </c>
+      <c r="Z84">
+        <v>227860</v>
+      </c>
+      <c r="AA84">
+        <v>13037</v>
+      </c>
+      <c r="AB84">
+        <v>246760</v>
+      </c>
+      <c r="AC84">
+        <v>709592</v>
+      </c>
+      <c r="AD84">
+        <v>9449</v>
+      </c>
+      <c r="AE84">
+        <v>919204</v>
+      </c>
+      <c r="AF84">
+        <v>60243</v>
+      </c>
+      <c r="AG84">
+        <v>56035</v>
+      </c>
+      <c r="AH84">
+        <v>542972</v>
+      </c>
+      <c r="AI84">
+        <v>56724</v>
+      </c>
+      <c r="AJ84">
+        <v>410854</v>
+      </c>
+      <c r="AK84">
+        <v>7967311</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>